<commit_message>
change in excel path and updated excel
</commit_message>
<xml_diff>
--- a/data/contest.xlsx
+++ b/data/contest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
   <si>
     <t>Match_no</t>
   </si>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -801,6 +801,29 @@
       </c>
       <c r="G17">
         <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>